<commit_message>
1. Set font in 'write_cell_content' func; 2. Get data only from excel cell.
</commit_message>
<xml_diff>
--- a/test_data/test_data.xlsx
+++ b/test_data/test_data.xlsx
@@ -8,28 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\data_driven_test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8DFE91-B537-4AC2-8E99-6732F90EFC81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8869C56B-E7F1-4DFD-B28F-6AA9E0D44958}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="account" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>序号</t>
   </si>
@@ -73,34 +65,46 @@
     <t>执行时间</t>
   </si>
   <si>
-    <t>jessicatest20200721001</t>
+    <t>jessicatest202007211</t>
+  </si>
+  <si>
+    <t>202007211</t>
   </si>
   <si>
     <t>Hot</t>
   </si>
   <si>
-    <t>Account "jessicatest20200721001" was created.</t>
-  </si>
-  <si>
-    <t>jessicatest20200721002</t>
+    <t>Account "jessicatest202007211" was created.</t>
+  </si>
+  <si>
+    <t>jessicatest202007212</t>
+  </si>
+  <si>
+    <t>202007212</t>
   </si>
   <si>
     <t>Warm</t>
   </si>
   <si>
-    <t>Account "jessicatest20200721002" was created.</t>
+    <t>Account "jessicatest202007212" was created.</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>jessicatest20200721003</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>jessicatest202007213</t>
+  </si>
+  <si>
+    <t>202007213</t>
   </si>
   <si>
     <t>Cold</t>
   </si>
   <si>
-    <t>Account "jessicatest20200721003" was created.</t>
+    <t>Account "jessicatest202007213" was created.</t>
   </si>
   <si>
     <t>passwordtest</t>
@@ -110,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +129,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF3030"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,9 +157,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -434,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -476,14 +486,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="str">
-        <f>IF(UPPER(E2)="N","NA","")</f>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -502,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -552,37 +558,41 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
-        <v>20200721001</v>
+      <c r="C2" t="s">
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>20200721002</v>
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -590,20 +600,21 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>20200721003</v>
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
+      <c r="H4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create functions to get valid data range in excel and store it as a list, each valid row is stored as a dict in the list.
</commit_message>
<xml_diff>
--- a/test_data/test_data.xlsx
+++ b/test_data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\data_driven_test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8869C56B-E7F1-4DFD-B28F-6AA9E0D44958}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F827CFC-8238-451D-ADC9-D30E80C1A75F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +134,12 @@
       <sz val="11"/>
       <color rgb="FFFF3030"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -508,7 +514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -617,6 +625,7 @@
       <c r="H4" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>